<commit_message>
added writing to excel for GR method
</commit_message>
<xml_diff>
--- a/01-lab/results/excel/bisection_method.xlsx
+++ b/01-lab/results/excel/bisection_method.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr date1904="false" showObjects="all" backupFile="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -10,7 +10,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr fullCalcOnLoad="true" refMode="A1" iterate="false" iterateCount="100" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
@@ -56,7 +56,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -64,6 +64,7 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -90,7 +91,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -99,6 +100,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -112,44 +114,44 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+<a:theme xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="LibreOffice">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="18a303"/>
+        <a:srgbClr val="18A303"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="0369a3"/>
+        <a:srgbClr val="0369A3"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="a33e03"/>
+        <a:srgbClr val="A33E03"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8e03a3"/>
+        <a:srgbClr val="8E03A3"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="c99c00"/>
+        <a:srgbClr val="C99C00"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="c9211e"/>
+        <a:srgbClr val="C9211E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000ee"/>
+        <a:srgbClr val="0000EE"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="551a8b"/>
+        <a:srgbClr val="551A8B"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
@@ -218,7 +220,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -230,320 +232,324 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="0" width="14.41"/>
+    <col min="1" max="1" width="8.7109375" style="0" hidden="false" customWidth="true" outlineLevel="0" collapsed="false"/>
+    <col min="2" max="2" width="8.7109375" style="0" hidden="false" customWidth="true" outlineLevel="0" collapsed="false"/>
+    <col min="3" max="3" width="8.7109375" style="0" hidden="false" customWidth="true" outlineLevel="0" collapsed="false"/>
+    <col min="4" max="4" width="8.7109375" style="0" hidden="false" customWidth="true" outlineLevel="0" collapsed="false"/>
+    <col min="5" max="5" width="9.7109375" style="0" hidden="false" customWidth="true" outlineLevel="0" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="n">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
         <v>2.5</v>
       </c>
-      <c r="C1" s="1" t="n">
+      <c r="C1" s="1">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="n">
+      <c r="D1" s="1">
         <v>7.5</v>
       </c>
-      <c r="E1" s="1" t="n">
+      <c r="E1" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="n">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
         <v>1.25</v>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="C2" s="1">
         <v>2.5</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="1">
         <v>3.75</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="E2" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="n">
+      <c r="A3" s="1">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1">
         <v>0.625</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" s="1">
         <v>1.25</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="1">
         <v>1.875</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="E3" s="1">
         <v>2.5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+      <c r="A4" s="1">
         <v>0.625</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="1">
         <v>0.9375</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="C4" s="1">
         <v>1.25</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4" s="1">
         <v>1.5625</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="E4" s="1">
         <v>1.875</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+      <c r="A5" s="1">
         <v>0.625</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B5" s="1">
         <v>0.78125</v>
       </c>
-      <c r="C5" s="1" t="n">
+      <c r="C5" s="1">
         <v>0.9375</v>
       </c>
-      <c r="D5" s="1" t="n">
+      <c r="D5" s="1">
         <v>1.09375</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="E5" s="1">
         <v>1.25</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
+      <c r="A6" s="1">
         <v>0.78125</v>
       </c>
-      <c r="B6" s="1" t="n">
+      <c r="B6" s="1">
         <v>0.859375</v>
       </c>
-      <c r="C6" s="1" t="n">
+      <c r="C6" s="1">
         <v>0.9375</v>
       </c>
-      <c r="D6" s="1" t="n">
+      <c r="D6" s="1">
         <v>1.015625</v>
       </c>
-      <c r="E6" s="1" t="n">
+      <c r="E6" s="1">
         <v>1.09375</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
+      <c r="A7" s="1">
         <v>0.9375</v>
       </c>
-      <c r="B7" s="1" t="n">
+      <c r="B7" s="1">
         <v>0.9765625</v>
       </c>
-      <c r="C7" s="1" t="n">
+      <c r="C7" s="1">
         <v>1.015625</v>
       </c>
-      <c r="D7" s="1" t="n">
+      <c r="D7" s="1">
         <v>1.0546875</v>
       </c>
-      <c r="E7" s="1" t="n">
+      <c r="E7" s="1">
         <v>1.09375</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
+      <c r="A8" s="1">
         <v>0.9765625</v>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="B8" s="1">
         <v>0.99609375</v>
       </c>
-      <c r="C8" s="1" t="n">
+      <c r="C8" s="1">
         <v>1.015625</v>
       </c>
-      <c r="D8" s="1" t="n">
+      <c r="D8" s="1">
         <v>1.03515625</v>
       </c>
-      <c r="E8" s="1" t="n">
+      <c r="E8" s="1">
         <v>1.0546875</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
+      <c r="A9" s="1">
         <v>0.9765625</v>
       </c>
-      <c r="B9" s="1" t="n">
+      <c r="B9" s="1">
         <v>0.986328125</v>
       </c>
-      <c r="C9" s="1" t="n">
+      <c r="C9" s="1">
         <v>0.99609375</v>
       </c>
-      <c r="D9" s="1" t="n">
+      <c r="D9" s="1">
         <v>1.005859375</v>
       </c>
-      <c r="E9" s="1" t="n">
+      <c r="E9" s="1">
         <v>1.015625</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
+      <c r="A10" s="1">
         <v>0.986328125</v>
       </c>
-      <c r="B10" s="1" t="n">
+      <c r="B10" s="1">
         <v>0.9912109375</v>
       </c>
-      <c r="C10" s="1" t="n">
+      <c r="C10" s="1">
         <v>0.99609375</v>
       </c>
-      <c r="D10" s="1" t="n">
+      <c r="D10" s="1">
         <v>1.0009765625</v>
       </c>
-      <c r="E10" s="1" t="n">
+      <c r="E10" s="1">
         <v>1.005859375</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
+      <c r="A11" s="1">
         <v>0.99609375</v>
       </c>
-      <c r="B11" s="1" t="n">
+      <c r="B11" s="1">
         <v>0.99853515625</v>
       </c>
-      <c r="C11" s="1" t="n">
+      <c r="C11" s="1">
         <v>1.0009765625</v>
       </c>
-      <c r="D11" s="1" t="n">
+      <c r="D11" s="1">
         <v>1.00341796875</v>
       </c>
-      <c r="E11" s="1" t="n">
+      <c r="E11" s="1">
         <v>1.005859375</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
+      <c r="A12" s="1">
         <v>0.99853515625</v>
       </c>
-      <c r="B12" s="1" t="n">
+      <c r="B12" s="1">
         <v>0.999755859375</v>
       </c>
-      <c r="C12" s="1" t="n">
+      <c r="C12" s="1">
         <v>1.0009765625</v>
       </c>
-      <c r="D12" s="1" t="n">
+      <c r="D12" s="1">
         <v>1.002197265625</v>
       </c>
-      <c r="E12" s="1" t="n">
+      <c r="E12" s="1">
         <v>1.00341796875</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
+      <c r="A13" s="1">
         <v>0.99853515625</v>
       </c>
-      <c r="B13" s="1" t="n">
+      <c r="B13" s="1">
         <v>0.9991455078125</v>
       </c>
-      <c r="C13" s="1" t="n">
+      <c r="C13" s="1">
         <v>0.999755859375</v>
       </c>
-      <c r="D13" s="1" t="n">
+      <c r="D13" s="1">
         <v>1.0003662109375</v>
       </c>
-      <c r="E13" s="1" t="n">
+      <c r="E13" s="1">
         <v>1.0009765625</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
+      <c r="A14" s="1">
         <v>0.9991455078125</v>
       </c>
-      <c r="B14" s="1" t="n">
+      <c r="B14" s="1">
         <v>0.99945068359375</v>
       </c>
-      <c r="C14" s="1" t="n">
+      <c r="C14" s="1">
         <v>0.999755859375</v>
       </c>
-      <c r="D14" s="1" t="n">
+      <c r="D14" s="1">
         <v>1.00006103515625</v>
       </c>
-      <c r="E14" s="1" t="n">
+      <c r="E14" s="1">
         <v>1.0003662109375</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="n">
+      <c r="A15" s="1">
         <v>0.999755859375</v>
       </c>
-      <c r="B15" s="1" t="n">
+      <c r="B15" s="1">
         <v>0.999908447265625</v>
       </c>
-      <c r="C15" s="1" t="n">
+      <c r="C15" s="1">
         <v>1.00006103515625</v>
       </c>
-      <c r="D15" s="1" t="n">
-        <v>1.00021362304688</v>
-      </c>
-      <c r="E15" s="1" t="n">
+      <c r="D15" s="1">
+        <v>1.000213623046875</v>
+      </c>
+      <c r="E15" s="1">
         <v>1.0003662109375</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
+      <c r="A16" s="1">
         <v>0.999908447265625</v>
       </c>
-      <c r="B16" s="1" t="n">
-        <v>0.999984741210938</v>
-      </c>
-      <c r="C16" s="1" t="n">
+      <c r="B16" s="1">
+        <v>0.9999847412109375</v>
+      </c>
+      <c r="C16" s="1">
         <v>1.00006103515625</v>
       </c>
-      <c r="D16" s="1" t="n">
-        <v>1.00013732910156</v>
-      </c>
-      <c r="E16" s="1" t="n">
-        <v>1.00021362304688</v>
+      <c r="D16" s="1">
+        <v>1.0001373291015625</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1.000213623046875</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="n">
+      <c r="A17" s="1">
         <v>0.999908447265625</v>
       </c>
-      <c r="B17" s="1" t="n">
-        <v>0.999946594238281</v>
-      </c>
-      <c r="C17" s="1" t="n">
-        <v>0.999984741210938</v>
-      </c>
-      <c r="D17" s="1" t="n">
-        <v>1.00002288818359</v>
-      </c>
-      <c r="E17" s="1" t="n">
+      <c r="B17" s="1">
+        <v>0.99994659423828125</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.9999847412109375</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1.0000228881835938</v>
+      </c>
+      <c r="E17" s="1">
         <v>1.00006103515625</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B18" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C18" s="1" t="n">
-        <v>0.999984741210938</v>
-      </c>
-      <c r="D18" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E18" s="1" t="n">
+      <c r="A18" s="1">
+        <v>0</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.9999847412109375</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <printOptions horizontalCentered="false" verticalCentered="false" headings="false" gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="0.74791666666667" right="0.74791666666667" top="0.98402777777778" bottom="0.98402777777778" header="0.51181102362205" footer="0.51181102362205"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <headerFooter differentOddEven="false" differentFirst="false">
     <oddHeader/>
     <oddFooter/>
   </headerFooter>

</xml_diff>

<commit_message>
more informative graph for Newton's method
</commit_message>
<xml_diff>
--- a/01-lab/results/excel/bisection_method.xlsx
+++ b/01-lab/results/excel/bisection_method.xlsx
@@ -17,6 +17,86 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="29" uniqueCount="25">
+  <si>
+    <t xml:space="preserve">l</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x_m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 iteracija</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 iteracija</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 iteracija</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 iteracija</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 iteracija</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 iteracija</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 iteracija</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 iteracija</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 iteracija</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 iteracija</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 iteracija</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 iteracija</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13 iteracija</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 iteracija</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 iteracija</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 iteracija</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17 iteracija</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18 iteracija</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -91,13 +171,29 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
@@ -224,325 +320,475 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
+      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="0" hidden="false" customWidth="true" outlineLevel="0" collapsed="false"/>
-    <col min="2" max="2" width="8.7109375" style="0" hidden="false" customWidth="true" outlineLevel="0" collapsed="false"/>
-    <col min="3" max="3" width="8.7109375" style="0" hidden="false" customWidth="true" outlineLevel="0" collapsed="false"/>
-    <col min="4" max="4" width="8.7109375" style="0" hidden="false" customWidth="true" outlineLevel="0" collapsed="false"/>
-    <col min="5" max="5" width="9.7109375" style="0" hidden="false" customWidth="true" outlineLevel="0" collapsed="false"/>
+    <col min="1" max="1" width="8.7109375" style="1" hidden="false" customWidth="true" outlineLevel="0" collapsed="false"/>
+    <col min="7" max="7" width="14.41" style="0" hidden="false" customWidth="true" outlineLevel="0" collapsed="false"/>
+    <col min="2" max="2" width="8.7109375" style="1" hidden="false" customWidth="true" outlineLevel="0" collapsed="false"/>
+    <col min="3" max="3" width="8.7109375" style="1" hidden="false" customWidth="true" outlineLevel="0" collapsed="false"/>
+    <col min="4" max="4" width="8.7109375" style="1" hidden="false" customWidth="true" outlineLevel="0" collapsed="false"/>
+    <col min="5" max="5" width="9.7109375" style="1" hidden="false" customWidth="true" outlineLevel="0" collapsed="false"/>
+    <col min="6" max="6" width="14.41" style="1" hidden="false" customWidth="true" outlineLevel="0" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1">
+      <c r="A1" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
+      <c r="B1" s="2">
         <v>2.5</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C1" s="2">
         <v>5</v>
       </c>
-      <c r="D1" s="1">
+      <c r="D1" s="2">
         <v>7.5</v>
       </c>
-      <c r="E1" s="1">
+      <c r="E1" s="2">
         <v>10</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1">
+      <c r="A2" s="4">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>1.25</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>2.5</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="2">
         <v>3.75</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="2">
         <v>5</v>
       </c>
+      <c r="F2" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2" s="3" t="n">
+        <f aca="false"> F2-B2</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1">
+      <c r="A3" s="4">
         <v>0</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>0.625</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="2">
         <v>1.25</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="2">
         <v>1.875</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="2">
         <v>2.5</v>
       </c>
+      <c r="F3" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="G3" s="3" t="n">
+        <f aca="false"> F3-B3</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1">
+      <c r="A4" s="4">
         <v>0.625</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="2">
         <v>0.9375</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="2">
         <v>1.25</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="2">
         <v>1.5625</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="2">
         <v>1.875</v>
       </c>
+      <c r="F4" s="2" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="G4" s="3" t="n">
+        <f aca="false"> F4-B4</f>
+        <v>2.5</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1">
+      <c r="A5" s="4">
         <v>0.625</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="2">
         <v>0.78125</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="2">
         <v>0.9375</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="2">
         <v>1.09375</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="2">
         <v>1.25</v>
       </c>
+      <c r="F5" s="2" t="n">
+        <v>1.875</v>
+      </c>
+      <c r="G5" s="3" t="n">
+        <f aca="false"> F5-B5</f>
+        <v>1.25</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1">
+      <c r="A6" s="4">
         <v>0.78125</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="2">
         <v>0.859375</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="2">
         <v>0.9375</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="2">
         <v>1.015625</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="2">
         <v>1.09375</v>
       </c>
+      <c r="F6" s="2" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="G6" s="3" t="n">
+        <f aca="false"> F6-B6</f>
+        <v>0.625</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1">
+      <c r="A7" s="4">
         <v>0.9375</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="2">
         <v>0.9765625</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="2">
         <v>1.015625</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="2">
         <v>1.0546875</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="2">
         <v>1.09375</v>
       </c>
+      <c r="F7" s="2" t="n">
+        <v>1.09375</v>
+      </c>
+      <c r="G7" s="3" t="n">
+        <f aca="false"> F7-B7</f>
+        <v>0.3125</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1">
+      <c r="A8" s="4">
         <v>0.9765625</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="2">
         <v>0.99609375</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="2">
         <v>1.015625</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="2">
         <v>1.03515625</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="2">
         <v>1.0546875</v>
       </c>
+      <c r="F8" s="2" t="n">
+        <v>1.09375</v>
+      </c>
+      <c r="G8" s="3" t="n">
+        <f aca="false"> F8-B8</f>
+        <v>0.15625</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1">
+      <c r="A9" s="4">
         <v>0.9765625</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="2">
         <v>0.986328125</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="2">
         <v>0.99609375</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="2">
         <v>1.005859375</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="2">
         <v>1.015625</v>
       </c>
+      <c r="F9" s="2" t="n">
+        <v>1.0546875</v>
+      </c>
+      <c r="G9" s="3" t="n">
+        <f aca="false"> F9-B9</f>
+        <v>0.078125</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1">
+      <c r="A10" s="4">
         <v>0.986328125</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="2">
         <v>0.9912109375</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="2">
         <v>0.99609375</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="2">
         <v>1.0009765625</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="2">
         <v>1.005859375</v>
       </c>
+      <c r="F10" s="2" t="n">
+        <v>1.015625</v>
+      </c>
+      <c r="G10" s="3" t="n">
+        <f aca="false"> F10-B10</f>
+        <v>0.0390625</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1">
+      <c r="A11" s="4">
         <v>0.99609375</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="2">
         <v>0.99853515625</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="2">
         <v>1.0009765625</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="2">
         <v>1.00341796875</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="2">
         <v>1.005859375</v>
       </c>
+      <c r="F11" s="2" t="n">
+        <v>1.005859375</v>
+      </c>
+      <c r="G11" s="3" t="n">
+        <f aca="false"> F11-B11</f>
+        <v>0.01953125</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1">
+      <c r="A12" s="4">
         <v>0.99853515625</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="2">
         <v>0.999755859375</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="2">
         <v>1.0009765625</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="2">
         <v>1.002197265625</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="2">
         <v>1.00341796875</v>
       </c>
+      <c r="F12" s="2" t="n">
+        <v>1.005859375</v>
+      </c>
+      <c r="G12" s="3" t="n">
+        <f aca="false"> F12-B12</f>
+        <v>0.009765625</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1">
+      <c r="A13" s="4">
         <v>0.99853515625</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="2">
         <v>0.9991455078125</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="2">
         <v>0.999755859375</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="2">
         <v>1.0003662109375</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="2">
         <v>1.0009765625</v>
       </c>
+      <c r="F13" s="2" t="n">
+        <v>1.00341796875</v>
+      </c>
+      <c r="G13" s="3" t="n">
+        <f aca="false"> F13-B13</f>
+        <v>0.0048828125</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1">
+      <c r="A14" s="4">
         <v>0.9991455078125</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="2">
         <v>0.99945068359375</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="2">
         <v>0.999755859375</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="2">
         <v>1.00006103515625</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="2">
         <v>1.0003662109375</v>
       </c>
+      <c r="F14" s="2" t="n">
+        <v>1.0009765625</v>
+      </c>
+      <c r="G14" s="3" t="n">
+        <f aca="false"> F14-B14</f>
+        <v>0.00244140625</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1">
+      <c r="A15" s="4">
         <v>0.999755859375</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="2">
         <v>0.999908447265625</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="2">
         <v>1.00006103515625</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="2">
         <v>1.000213623046875</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="2">
         <v>1.0003662109375</v>
       </c>
+      <c r="F15" s="2" t="n">
+        <v>1.0003662109375</v>
+      </c>
+      <c r="G15" s="3" t="n">
+        <f aca="false"> F15-B15</f>
+        <v>0.001220703125</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1">
+      <c r="A16" s="4">
         <v>0.999908447265625</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="2">
         <v>0.9999847412109375</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="2">
         <v>1.00006103515625</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="2">
         <v>1.0001373291015625</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="2">
         <v>1.000213623046875</v>
       </c>
+      <c r="F16" s="2" t="n">
+        <v>1.0003662109375</v>
+      </c>
+      <c r="G16" s="3" t="n">
+        <f aca="false"> F16-B16</f>
+        <v>0.0006103515625</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1">
+      <c r="A17" s="4">
         <v>0.999908447265625</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="2">
         <v>0.99994659423828125</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="2">
         <v>0.9999847412109375</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="2">
         <v>1.0000228881835938</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="2">
         <v>1.00006103515625</v>
       </c>
+      <c r="F17" s="2" t="n">
+        <v>1.00021362304688</v>
+      </c>
+      <c r="G17" s="3" t="n">
+        <f aca="false"> F17-B17</f>
+        <v>0.000305175781255107</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1">
+      <c r="A18" s="4">
         <v>0</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="2">
         <v>0</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="2">
         <v>0.9999847412109375</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="2">
         <v>0</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="2">
         <v>0</v>
+      </c>
+      <c r="F18" s="2" t="n">
+        <v>1.00006103515625</v>
+      </c>
+      <c r="G18" s="3" t="n">
+        <f aca="false"> F18-B18</f>
+        <v>0.000152587890625</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>0.999984741210938</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>